<commit_message>
termino de importacion de orientacion espacial
</commit_message>
<xml_diff>
--- a/orientacion espacial.xlsx
+++ b/orientacion espacial.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t xml:space="preserve">question_image</t>
   </si>
@@ -46,7 +46,19 @@
     <t xml:space="preserve">feedback_image</t>
   </si>
   <si>
+    <t xml:space="preserve">A</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lorem ipsum dolor sit amet, consectetur adipiscing elit. Morbi eget viverra ipsum. Nam dolor libero, ullamcorper quis dolor vitae, semper tristique augue.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
   </si>
 </sst>
 </file>
@@ -61,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -81,6 +94,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -125,12 +139,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -157,9 +175,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
+      <xdr:colOff>166680</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>144360</xdr:rowOff>
+      <xdr:rowOff>170280</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -173,7 +191,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="162720"/>
-          <a:ext cx="141480" cy="144360"/>
+          <a:ext cx="166680" cy="170280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -195,9 +213,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>126720</xdr:colOff>
+      <xdr:colOff>126360</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>133200</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -211,7 +229,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="356760"/>
-          <a:ext cx="126720" cy="133200"/>
+          <a:ext cx="126360" cy="132840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -233,9 +251,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>134280</xdr:colOff>
+      <xdr:colOff>133920</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -249,7 +267,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="537120"/>
-          <a:ext cx="134280" cy="140400"/>
+          <a:ext cx="133920" cy="140040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -271,9 +289,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>141480</xdr:colOff>
+      <xdr:colOff>141120</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>142200</xdr:rowOff>
+      <xdr:rowOff>141840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -287,7 +305,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="717480"/>
-          <a:ext cx="141480" cy="142200"/>
+          <a:ext cx="141120" cy="141840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -309,9 +327,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>138960</xdr:colOff>
+      <xdr:colOff>138600</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>140400</xdr:rowOff>
+      <xdr:rowOff>140040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -325,7 +343,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="880200"/>
-          <a:ext cx="138960" cy="140400"/>
+          <a:ext cx="138600" cy="140040"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -347,9 +365,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>169560</xdr:colOff>
+      <xdr:colOff>169200</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:rowOff>172800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -362,8 +380,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5862240" y="162720"/>
-          <a:ext cx="169560" cy="173160"/>
+          <a:off x="5862960" y="162720"/>
+          <a:ext cx="169200" cy="172800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -385,9 +403,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>148320</xdr:colOff>
+      <xdr:colOff>147960</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>155520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -400,8 +418,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5862240" y="356760"/>
-          <a:ext cx="148320" cy="155880"/>
+          <a:off x="5862960" y="356760"/>
+          <a:ext cx="147960" cy="155520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -423,9 +441,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>127800</xdr:colOff>
+      <xdr:colOff>127440</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -438,8 +456,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5862240" y="717480"/>
-          <a:ext cx="127800" cy="133560"/>
+          <a:off x="5862960" y="717480"/>
+          <a:ext cx="127440" cy="133200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -568,136 +586,136 @@
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.63"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F3" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F4" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>8</v>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F5" s="0" t="n">
-        <v>4</v>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F6" s="0" t="n">
-        <v>1</v>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>